<commit_message>
Lack of comparison method and conclusion
must be finished before 23/05 5PM
</commit_message>
<xml_diff>
--- a/Lab2Data.xlsx
+++ b/Lab2Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>reference</t>
   </si>
@@ -99,6 +99,73 @@
   <si>
     <t>10
 [dB(A)]</t>
+  </si>
+  <si>
+    <t>T60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_pm  </t>
+  </si>
+  <si>
+    <t>T10 [s]</t>
+  </si>
+  <si>
+    <t>Frequency [Hz]</t>
+  </si>
+  <si>
+    <t>T20 [s]</t>
+  </si>
+  <si>
+    <t>T30 [s]</t>
+  </si>
+  <si>
+    <t>T60 [s]</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Frequency
+[Hz]</t>
+  </si>
+  <si>
+    <t>T60
+[s]</t>
+  </si>
+  <si>
+    <t>A
+[m^2]</t>
+  </si>
+  <si>
+    <t>K
+[dB(A)]</t>
+  </si>
+  <si>
+    <t>L_pm
+[dB(A)]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_pf
+[dB(A)]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L_w
+[dB(A)]  </t>
+  </si>
+  <si>
+    <t>L_w_unc</t>
+  </si>
+  <si>
+    <t>L_w</t>
   </si>
 </sst>
 </file>
@@ -114,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,8 +194,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -387,11 +466,204 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -445,6 +717,127 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -706,32 +1099,10 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -750,6 +1121,28 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -760,8 +1153,1013 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$28:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$28:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.1399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="76777344"/>
+        <c:axId val="76775808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="76777344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="76775808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="76775808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="76777344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$28:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$28:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="80374400"/>
+        <c:axId val="80372480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="80374400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80372480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="80372480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80374400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$28:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$28:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="80794752"/>
+        <c:axId val="80784768"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="80794752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80784768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="80784768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80794752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$28:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$28:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="82283136"/>
+        <c:axId val="82281600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="82283136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82281600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="82281600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82283136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11550240594925634"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.57421872265966756"/>
+          <c:h val="0.8326195683872849"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$28:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$28:$F$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="81636736"/>
+        <c:axId val="81635200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="81636736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81635200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="81635200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81636736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-AU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$28:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$28:$G$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="103965824"/>
+        <c:axId val="103959936"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="103965824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="103959936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="103959936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="103965824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A15:K22" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A15:K22" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A15:K22"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Column1" dataDxfId="10"/>
@@ -1067,36 +2465,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K22"/>
+  <dimension ref="A2:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:K22"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="11" customWidth="1"/>
     <col min="10" max="11" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -1127,8 +2525,17 @@
       <c r="K3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>125</v>
       </c>
@@ -1162,8 +2569,19 @@
       <c r="K4">
         <v>50.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="23">
+        <f>10*LOG((10^(0.1*B4)+10^(0.1*C4)+10^(0.1*D4)+10^(0.1*E4)+10^(0.1*F4)+10^(0.1*G4)+10^(0.1*H4)+10^(0.1*I4)+10^(0.1*J4)+10^(0.1*K4))/10,10)</f>
+        <v>51.581004998545254</v>
+      </c>
+      <c r="N4" s="23">
+        <f>M4+10*LOG(6.28,10)</f>
+        <v>59.560601435917214</v>
+      </c>
+      <c r="O4">
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>250</v>
       </c>
@@ -1197,8 +2615,19 @@
       <c r="K5">
         <v>58.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="23">
+        <f t="shared" ref="M5:M9" si="0">10*LOG((10^(0.1*B5)+10^(0.1*C5)+10^(0.1*D5)+10^(0.1*E5)+10^(0.1*F5)+10^(0.1*G5)+10^(0.1*H5)+10^(0.1*I5)+10^(0.1*J5)+10^(0.1*K5))/10,10)</f>
+        <v>60.086941440787207</v>
+      </c>
+      <c r="N5" s="23">
+        <f t="shared" ref="N5:N9" si="1">M5+10*LOG(6.28,10)</f>
+        <v>68.066537878159167</v>
+      </c>
+      <c r="O5">
+        <v>82.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>500</v>
       </c>
@@ -1232,8 +2661,19 @@
       <c r="K6">
         <v>63.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="23">
+        <f t="shared" si="0"/>
+        <v>65.036543226804142</v>
+      </c>
+      <c r="N6" s="23">
+        <f t="shared" si="1"/>
+        <v>73.016139664176109</v>
+      </c>
+      <c r="O6">
+        <v>82.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1000</v>
       </c>
@@ -1267,8 +2707,19 @@
       <c r="K7">
         <v>75.099999999999994</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="23">
+        <f t="shared" si="0"/>
+        <v>73.806493137932776</v>
+      </c>
+      <c r="N7" s="23">
+        <f t="shared" si="1"/>
+        <v>81.786089575304743</v>
+      </c>
+      <c r="O7">
+        <v>87.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2000</v>
       </c>
@@ -1302,8 +2753,19 @@
       <c r="K8">
         <v>75.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="23">
+        <f t="shared" si="0"/>
+        <v>75.744427755347786</v>
+      </c>
+      <c r="N8" s="23">
+        <f t="shared" si="1"/>
+        <v>83.724024192719753</v>
+      </c>
+      <c r="O8">
+        <v>86.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3150</v>
       </c>
@@ -1337,23 +2799,34 @@
       <c r="K9">
         <v>71</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="M9" s="23">
+        <f t="shared" si="0"/>
+        <v>72.235855199944524</v>
+      </c>
+      <c r="N9" s="23">
+        <f t="shared" si="1"/>
+        <v>80.215451637316491</v>
+      </c>
+      <c r="O9">
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1388,7 +2861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
@@ -1422,8 +2895,11 @@
       <c r="K16" s="15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>125</v>
       </c>
@@ -1457,8 +2933,12 @@
       <c r="K17" s="16">
         <v>29.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M17" s="23">
+        <f>10*LOG((10^(0.1*Table2[[#This Row],[Column2]])+10^(0.1*Table2[[#This Row],[Column3]])+10^(0.1*Table2[[#This Row],[Column4]])+10^(0.1*Table2[[#This Row],[Column5]])+10^(0.1*Table2[[#This Row],[Column6]])+10^(0.1*Table2[[#This Row],[Column7]])+10^(0.1*Table2[[#This Row],[Column8]])+10^(0.1*Table2[[#This Row],[Column9]])+10^(0.1*Table2[[#This Row],[Column10]])+10^(0.1*Table2[[#This Row],[Column11]]))/10,10)</f>
+        <v>36.829681899252094</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>250</v>
       </c>
@@ -1492,8 +2972,12 @@
       <c r="K18" s="17">
         <v>31.8</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M18" s="23">
+        <f>10*LOG((10^(0.1*Table2[[#This Row],[Column2]])+10^(0.1*Table2[[#This Row],[Column3]])+10^(0.1*Table2[[#This Row],[Column4]])+10^(0.1*Table2[[#This Row],[Column5]])+10^(0.1*Table2[[#This Row],[Column6]])+10^(0.1*Table2[[#This Row],[Column7]])+10^(0.1*Table2[[#This Row],[Column8]])+10^(0.1*Table2[[#This Row],[Column9]])+10^(0.1*Table2[[#This Row],[Column10]])+10^(0.1*Table2[[#This Row],[Column11]]))/10,10)</f>
+        <v>33.242390994024916</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>500</v>
       </c>
@@ -1527,8 +3011,12 @@
       <c r="K19" s="17">
         <v>37.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M19" s="23">
+        <f>10*LOG((10^(0.1*Table2[[#This Row],[Column2]])+10^(0.1*Table2[[#This Row],[Column3]])+10^(0.1*Table2[[#This Row],[Column4]])+10^(0.1*Table2[[#This Row],[Column5]])+10^(0.1*Table2[[#This Row],[Column6]])+10^(0.1*Table2[[#This Row],[Column7]])+10^(0.1*Table2[[#This Row],[Column8]])+10^(0.1*Table2[[#This Row],[Column9]])+10^(0.1*Table2[[#This Row],[Column10]])+10^(0.1*Table2[[#This Row],[Column11]]))/10,10)</f>
+        <v>38.360938804620673</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>1000</v>
       </c>
@@ -1562,8 +3050,12 @@
       <c r="K20" s="17">
         <v>44.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20" s="23">
+        <f>10*LOG((10^(0.1*Table2[[#This Row],[Column2]])+10^(0.1*Table2[[#This Row],[Column3]])+10^(0.1*Table2[[#This Row],[Column4]])+10^(0.1*Table2[[#This Row],[Column5]])+10^(0.1*Table2[[#This Row],[Column6]])+10^(0.1*Table2[[#This Row],[Column7]])+10^(0.1*Table2[[#This Row],[Column8]])+10^(0.1*Table2[[#This Row],[Column9]])+10^(0.1*Table2[[#This Row],[Column10]])+10^(0.1*Table2[[#This Row],[Column11]]))/10,10)</f>
+        <v>46.684886395908222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>2000</v>
       </c>
@@ -1597,8 +3089,12 @@
       <c r="K21" s="17">
         <v>55.7</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M21" s="23">
+        <f>10*LOG((10^(0.1*Table2[[#This Row],[Column2]])+10^(0.1*Table2[[#This Row],[Column3]])+10^(0.1*Table2[[#This Row],[Column4]])+10^(0.1*Table2[[#This Row],[Column5]])+10^(0.1*Table2[[#This Row],[Column6]])+10^(0.1*Table2[[#This Row],[Column7]])+10^(0.1*Table2[[#This Row],[Column8]])+10^(0.1*Table2[[#This Row],[Column9]])+10^(0.1*Table2[[#This Row],[Column10]])+10^(0.1*Table2[[#This Row],[Column11]]))/10,10)</f>
+        <v>57.888548048435283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>3150</v>
       </c>
@@ -1631,6 +3127,760 @@
       </c>
       <c r="K22" s="20">
         <v>52.3</v>
+      </c>
+      <c r="M22" s="23">
+        <f>10*LOG((10^(0.1*Table2[[#This Row],[Column2]])+10^(0.1*Table2[[#This Row],[Column3]])+10^(0.1*Table2[[#This Row],[Column4]])+10^(0.1*Table2[[#This Row],[Column5]])+10^(0.1*Table2[[#This Row],[Column6]])+10^(0.1*Table2[[#This Row],[Column7]])+10^(0.1*Table2[[#This Row],[Column8]])+10^(0.1*Table2[[#This Row],[Column9]])+10^(0.1*Table2[[#This Row],[Column10]])+10^(0.1*Table2[[#This Row],[Column11]]))/10,10)</f>
+        <v>54.165215386170473</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22">
+        <v>125</v>
+      </c>
+      <c r="C27" s="22">
+        <v>250</v>
+      </c>
+      <c r="D27" s="22">
+        <v>500</v>
+      </c>
+      <c r="E27" s="22">
+        <v>1000</v>
+      </c>
+      <c r="F27" s="22">
+        <v>2000</v>
+      </c>
+      <c r="G27" s="22">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="22">
+        <v>10</v>
+      </c>
+      <c r="B28" s="22">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C28" s="22">
+        <v>1.81</v>
+      </c>
+      <c r="D28" s="22">
+        <v>1.73</v>
+      </c>
+      <c r="E28" s="22">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="F28" s="22">
+        <v>2.1</v>
+      </c>
+      <c r="G28" s="22">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="22">
+        <v>20</v>
+      </c>
+      <c r="B29" s="22">
+        <v>1.21</v>
+      </c>
+      <c r="C29" s="22">
+        <v>1.77</v>
+      </c>
+      <c r="D29" s="22">
+        <v>1.96</v>
+      </c>
+      <c r="E29" s="22">
+        <v>2.39</v>
+      </c>
+      <c r="F29" s="22">
+        <v>2.14</v>
+      </c>
+      <c r="G29" s="22">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="22">
+        <v>30</v>
+      </c>
+      <c r="B30" s="22">
+        <v>1.25</v>
+      </c>
+      <c r="C30" s="22">
+        <v>1.6</v>
+      </c>
+      <c r="D30" s="22">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E30" s="22">
+        <v>2.9</v>
+      </c>
+      <c r="F30" s="22">
+        <v>2.13</v>
+      </c>
+      <c r="G30" s="22">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="22">
+        <v>60</v>
+      </c>
+      <c r="B31" s="22">
+        <f>0.0055*A31+1.09</f>
+        <v>1.42</v>
+      </c>
+      <c r="C31" s="22">
+        <f>-0.0105*A31 + 1.9367</f>
+        <v>1.3067000000000002</v>
+      </c>
+      <c r="D31" s="22">
+        <f>0.014*A31 + 1.62</f>
+        <v>2.46</v>
+      </c>
+      <c r="E31" s="22">
+        <f xml:space="preserve"> 0.0425*A31 + 1.5967</f>
+        <v>4.1467000000000001</v>
+      </c>
+      <c r="F31" s="22">
+        <f xml:space="preserve"> 0.0015*A31 + 2.0933</f>
+        <v>2.1833</v>
+      </c>
+      <c r="G31" s="22">
+        <f xml:space="preserve"> 0.0135*A31 + 1.53</f>
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="25">
+        <v>125</v>
+      </c>
+      <c r="C34" s="25">
+        <v>250</v>
+      </c>
+      <c r="D34" s="25">
+        <v>500</v>
+      </c>
+      <c r="E34" s="25">
+        <v>1000</v>
+      </c>
+      <c r="F34" s="25">
+        <v>2000</v>
+      </c>
+      <c r="G34" s="26">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C35" s="4">
+        <v>1.81</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1.73</v>
+      </c>
+      <c r="E35" s="4">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="F35" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="G35" s="17">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1.21</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1.77</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1.96</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2.39</v>
+      </c>
+      <c r="F36" s="4">
+        <v>2.14</v>
+      </c>
+      <c r="G36" s="17">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="C37" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="D37" s="4">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="E37" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="F37" s="4">
+        <v>2.13</v>
+      </c>
+      <c r="G37" s="17">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="28">
+        <v>1.42</v>
+      </c>
+      <c r="C38" s="28">
+        <v>1.3067000000000002</v>
+      </c>
+      <c r="D38" s="28">
+        <v>2.46</v>
+      </c>
+      <c r="E38" s="28">
+        <v>4.1467000000000001</v>
+      </c>
+      <c r="F38" s="28">
+        <v>2.1833</v>
+      </c>
+      <c r="G38" s="29">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="32"/>
+    </row>
+    <row r="41" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I41" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="J41" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="K41" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="L41" s="51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>125</v>
+      </c>
+      <c r="B42" s="31">
+        <v>36.829681899252094</v>
+      </c>
+      <c r="C42" s="33">
+        <v>1.42</v>
+      </c>
+      <c r="D42" s="23">
+        <f>55.3*F42/G42/C42</f>
+        <v>59.948260994538657</v>
+      </c>
+      <c r="E42" s="23">
+        <f>10*LOG(1+4*6.28/D42,10)</f>
+        <v>1.5199096543059507</v>
+      </c>
+      <c r="F42" s="1">
+        <v>528</v>
+      </c>
+      <c r="G42" s="1">
+        <v>343</v>
+      </c>
+      <c r="I42" s="52">
+        <v>125</v>
+      </c>
+      <c r="J42" s="46">
+        <v>1.42</v>
+      </c>
+      <c r="K42" s="45">
+        <v>59.948260994538657</v>
+      </c>
+      <c r="L42" s="53">
+        <f>10*LOG(1+4*6.28/K42,10)</f>
+        <v>1.5199096543059507</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>250</v>
+      </c>
+      <c r="B43" s="31">
+        <v>33.242390994024916</v>
+      </c>
+      <c r="C43" s="33">
+        <v>1.3067000000000002</v>
+      </c>
+      <c r="D43" s="23">
+        <f t="shared" ref="D43:D47" si="2">55.3*F43/G43/C43</f>
+        <v>65.146193167708645</v>
+      </c>
+      <c r="E43" s="23">
+        <f t="shared" ref="E43:E47" si="3">10*LOG(1+4*6.28/D43,10)</f>
+        <v>1.4163608447555704</v>
+      </c>
+      <c r="F43" s="1">
+        <v>528</v>
+      </c>
+      <c r="G43" s="1">
+        <v>343</v>
+      </c>
+      <c r="I43" s="54">
+        <v>250</v>
+      </c>
+      <c r="J43" s="47">
+        <v>1.3067000000000002</v>
+      </c>
+      <c r="K43" s="33">
+        <v>65.146193167708645</v>
+      </c>
+      <c r="L43" s="55">
+        <f t="shared" ref="L43:L47" si="4">10*LOG(1+4*6.28/K43,10)</f>
+        <v>1.4163608447555704</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>500</v>
+      </c>
+      <c r="B44" s="31">
+        <v>38.360938804620673</v>
+      </c>
+      <c r="C44" s="33">
+        <v>2.46</v>
+      </c>
+      <c r="D44" s="23">
+        <f t="shared" si="2"/>
+        <v>34.604280736684913</v>
+      </c>
+      <c r="E44" s="23">
+        <f t="shared" si="3"/>
+        <v>2.3702110152495477</v>
+      </c>
+      <c r="F44" s="1">
+        <v>528</v>
+      </c>
+      <c r="G44" s="1">
+        <v>343</v>
+      </c>
+      <c r="I44" s="54">
+        <v>500</v>
+      </c>
+      <c r="J44" s="47">
+        <v>2.46</v>
+      </c>
+      <c r="K44" s="33">
+        <v>34.604280736684913</v>
+      </c>
+      <c r="L44" s="55">
+        <f t="shared" si="4"/>
+        <v>2.3702110152495477</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1000</v>
+      </c>
+      <c r="B45" s="31">
+        <v>46.684886395908222</v>
+      </c>
+      <c r="C45" s="33">
+        <v>4.1467000000000001</v>
+      </c>
+      <c r="D45" s="23">
+        <f t="shared" si="2"/>
+        <v>20.528741074166177</v>
+      </c>
+      <c r="E45" s="23">
+        <f t="shared" si="3"/>
+        <v>3.4706648776437179</v>
+      </c>
+      <c r="F45" s="1">
+        <v>528</v>
+      </c>
+      <c r="G45" s="1">
+        <v>343</v>
+      </c>
+      <c r="I45" s="54">
+        <v>1000</v>
+      </c>
+      <c r="J45" s="47">
+        <v>4.1467000000000001</v>
+      </c>
+      <c r="K45" s="33">
+        <v>20.528741074166177</v>
+      </c>
+      <c r="L45" s="55">
+        <f t="shared" si="4"/>
+        <v>3.4706648776437179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2000</v>
+      </c>
+      <c r="B46" s="31">
+        <v>57.888548048435283</v>
+      </c>
+      <c r="C46" s="33">
+        <v>2.1833</v>
+      </c>
+      <c r="D46" s="23">
+        <f t="shared" si="2"/>
+        <v>38.989845926920211</v>
+      </c>
+      <c r="E46" s="23">
+        <f t="shared" si="3"/>
+        <v>2.1597321413503168</v>
+      </c>
+      <c r="F46" s="1">
+        <v>528</v>
+      </c>
+      <c r="G46" s="1">
+        <v>343</v>
+      </c>
+      <c r="I46" s="54">
+        <v>2000</v>
+      </c>
+      <c r="J46" s="47">
+        <v>2.1833</v>
+      </c>
+      <c r="K46" s="33">
+        <v>38.989845926920211</v>
+      </c>
+      <c r="L46" s="55">
+        <f t="shared" si="4"/>
+        <v>2.1597321413503168</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>3150</v>
+      </c>
+      <c r="B47" s="31">
+        <v>54.165215386170473</v>
+      </c>
+      <c r="C47" s="33">
+        <v>2.34</v>
+      </c>
+      <c r="D47" s="23">
+        <f t="shared" si="2"/>
+        <v>36.378859236002093</v>
+      </c>
+      <c r="E47" s="23">
+        <f t="shared" si="3"/>
+        <v>2.2801798358324481</v>
+      </c>
+      <c r="F47" s="1">
+        <v>528</v>
+      </c>
+      <c r="G47" s="1">
+        <v>343</v>
+      </c>
+      <c r="I47" s="56">
+        <v>3150</v>
+      </c>
+      <c r="J47" s="57">
+        <v>2.34</v>
+      </c>
+      <c r="K47" s="58">
+        <v>36.378859236002093</v>
+      </c>
+      <c r="L47" s="59">
+        <f t="shared" si="4"/>
+        <v>2.2801798358324481</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G50" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="H50" s="36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="37">
+        <v>125</v>
+      </c>
+      <c r="C51" s="38">
+        <v>1.42</v>
+      </c>
+      <c r="D51" s="39">
+        <v>59.948260994538657</v>
+      </c>
+      <c r="E51" s="38">
+        <v>1.5199096543059507</v>
+      </c>
+      <c r="F51" s="39">
+        <v>36.829681899252094</v>
+      </c>
+      <c r="G51" s="40">
+        <f>F51-E51</f>
+        <v>35.309772244946146</v>
+      </c>
+      <c r="H51" s="23">
+        <f>G51+10*LOG(6.28,10)</f>
+        <v>43.289368682318106</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="37">
+        <v>250</v>
+      </c>
+      <c r="C52" s="38">
+        <v>1.3067000000000002</v>
+      </c>
+      <c r="D52" s="39">
+        <v>65.146193167708645</v>
+      </c>
+      <c r="E52" s="38">
+        <v>1.4163608447555704</v>
+      </c>
+      <c r="F52" s="39">
+        <v>33.242390994024916</v>
+      </c>
+      <c r="G52" s="40">
+        <f t="shared" ref="G52:G56" si="5">F52-E52</f>
+        <v>31.826030149269346</v>
+      </c>
+      <c r="H52" s="23">
+        <f t="shared" ref="H52:H56" si="6">G52+10*LOG(6.28,10)</f>
+        <v>39.80562658664131</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="37">
+        <v>500</v>
+      </c>
+      <c r="C53" s="38">
+        <v>2.46</v>
+      </c>
+      <c r="D53" s="39">
+        <v>34.604280736684913</v>
+      </c>
+      <c r="E53" s="38">
+        <v>2</v>
+      </c>
+      <c r="F53" s="39">
+        <v>38.360938804620673</v>
+      </c>
+      <c r="G53" s="40">
+        <f t="shared" si="5"/>
+        <v>36.360938804620673</v>
+      </c>
+      <c r="H53" s="23">
+        <f t="shared" si="6"/>
+        <v>44.340535241992633</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="37">
+        <v>1000</v>
+      </c>
+      <c r="C54" s="38">
+        <v>4.1467000000000001</v>
+      </c>
+      <c r="D54" s="39">
+        <v>20.528741074166177</v>
+      </c>
+      <c r="E54" s="38">
+        <v>2</v>
+      </c>
+      <c r="F54" s="39">
+        <v>46.684886395908222</v>
+      </c>
+      <c r="G54" s="40">
+        <f t="shared" si="5"/>
+        <v>44.684886395908222</v>
+      </c>
+      <c r="H54" s="23">
+        <f t="shared" si="6"/>
+        <v>52.664482833280182</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="37">
+        <v>2000</v>
+      </c>
+      <c r="C55" s="38">
+        <v>2.1833</v>
+      </c>
+      <c r="D55" s="39">
+        <v>38.989845926920211</v>
+      </c>
+      <c r="E55" s="38">
+        <v>2</v>
+      </c>
+      <c r="F55" s="39">
+        <v>57.888548048435283</v>
+      </c>
+      <c r="G55" s="40">
+        <f t="shared" si="5"/>
+        <v>55.888548048435283</v>
+      </c>
+      <c r="H55" s="23">
+        <f t="shared" si="6"/>
+        <v>63.868144485807242</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="41">
+        <v>3150</v>
+      </c>
+      <c r="C56" s="42">
+        <v>2.34</v>
+      </c>
+      <c r="D56" s="43">
+        <v>36.378859236002093</v>
+      </c>
+      <c r="E56" s="42">
+        <v>2</v>
+      </c>
+      <c r="F56" s="43">
+        <v>54.165215386170473</v>
+      </c>
+      <c r="G56" s="44">
+        <f t="shared" si="5"/>
+        <v>52.165215386170473</v>
+      </c>
+      <c r="H56" s="23">
+        <f t="shared" si="6"/>
+        <v>60.144811823542433</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E58" s="36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C59" s="60">
+        <v>125</v>
+      </c>
+      <c r="D59" s="38">
+        <v>35.309772244946146</v>
+      </c>
+      <c r="E59" s="62">
+        <v>43.289368682318106</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C60" s="60">
+        <v>250</v>
+      </c>
+      <c r="D60" s="38">
+        <v>31.826030149269346</v>
+      </c>
+      <c r="E60" s="62">
+        <v>39.80562658664131</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C61" s="60">
+        <v>500</v>
+      </c>
+      <c r="D61" s="38">
+        <v>36.360938804620673</v>
+      </c>
+      <c r="E61" s="62">
+        <v>44.340535241992633</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C62" s="60">
+        <v>1000</v>
+      </c>
+      <c r="D62" s="38">
+        <v>44.684886395908222</v>
+      </c>
+      <c r="E62" s="62">
+        <v>52.664482833280182</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C63" s="60">
+        <v>2000</v>
+      </c>
+      <c r="D63" s="38">
+        <v>55.888548048435283</v>
+      </c>
+      <c r="E63" s="62">
+        <v>63.868144485807242</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="61">
+        <v>3150</v>
+      </c>
+      <c r="D64" s="42">
+        <v>52.165215386170473</v>
+      </c>
+      <c r="E64" s="63">
+        <v>60.144811823542433</v>
       </c>
     </row>
   </sheetData>
@@ -1640,8 +3890,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>